<commit_message>
Scripts de Tablas e Inserts
</commit_message>
<xml_diff>
--- a/SQL/Modelo.xlsx
+++ b/SQL/Modelo.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java64\workspace\tp-patrones-persitidor\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBDF95C-8D46-49FE-8491-F6F1CB511474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01366622-5A34-4078-8C91-0C54336B708A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{1FA6D53A-2D3A-40AA-99BD-3A5E3626B78E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{1FA6D53A-2D3A-40AA-99BD-3A5E3626B78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sesion" sheetId="1" r:id="rId1"/>
-    <sheet name="Objeto" sheetId="5" r:id="rId2"/>
-    <sheet name="Clase" sheetId="2" r:id="rId3"/>
-    <sheet name="Atributo" sheetId="3" r:id="rId4"/>
-    <sheet name="Valor" sheetId="6" r:id="rId5"/>
-    <sheet name="Primitivo" sheetId="4" r:id="rId6"/>
+    <sheet name="Clase" sheetId="2" r:id="rId2"/>
+    <sheet name="Primitivo" sheetId="4" r:id="rId3"/>
+    <sheet name="Objeto" sheetId="5" r:id="rId4"/>
+    <sheet name="Atributo" sheetId="3" r:id="rId5"/>
+    <sheet name="Valor" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -732,6 +732,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6BD10E35-F03C-49D5-908E-2E5CEF5B3C92}" name="Tabla7" displayName="Tabla7" ref="A2:B4" totalsRowShown="0" dataDxfId="18">
+  <autoFilter ref="A2:B4" xr:uid="{6BD10E35-F03C-49D5-908E-2E5CEF5B3C92}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D8C413AE-6D4D-41A4-A5E4-E8086309B76A}" name="ID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{A9D4FA42-2751-4523-BCCA-576FE5F16CBB}" name="NOMBRE" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3EB20B64-F6DD-410D-8178-4BF665C122F3}" name="Tabla4" displayName="Tabla4" ref="A2:B11" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A2:B11" xr:uid="{3EB20B64-F6DD-410D-8178-4BF665C122F3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E2BFE1D0-31AA-4096-A1A9-1EC1DD7949F4}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{618BA1C2-FD69-4424-9500-69A5BC1723AC}" name="NOMBRE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3364FA21-105C-411A-BF6F-0EB60345DD01}" name="Tabla6" displayName="Tabla6" ref="A2:C6" totalsRowShown="0" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A2:C6" xr:uid="{3364FA21-105C-411A-BF6F-0EB60345DD01}"/>
   <tableColumns count="3">
@@ -743,18 +765,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6BD10E35-F03C-49D5-908E-2E5CEF5B3C92}" name="Tabla7" displayName="Tabla7" ref="A2:B4" totalsRowShown="0" dataDxfId="18">
-  <autoFilter ref="A2:B4" xr:uid="{6BD10E35-F03C-49D5-908E-2E5CEF5B3C92}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D8C413AE-6D4D-41A4-A5E4-E8086309B76A}" name="ID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{A9D4FA42-2751-4523-BCCA-576FE5F16CBB}" name="NOMBRE" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1A511366-58D6-4581-A75B-DEE2C3351E02}" name="Tabla5" displayName="Tabla5" ref="A2:F13" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="A2:F13" xr:uid="{1A511366-58D6-4581-A75B-DEE2C3351E02}"/>
   <tableColumns count="6">
@@ -769,7 +780,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F10132A3-C980-47B9-8FC3-1DC2AE879F9B}" name="Tabla8" displayName="Tabla8" ref="A2:E28" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A2:E28" xr:uid="{F10132A3-C980-47B9-8FC3-1DC2AE879F9B}"/>
   <tableColumns count="5">
@@ -778,17 +789,6 @@
     <tableColumn id="3" xr3:uid="{911EA243-45FC-42F3-8A79-EA995B705FD4}" name="ID_ATRIBUTO" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{377A820B-7800-438F-BCE4-E215D0FAC04B}" name="VALOR_PRIMITIVO" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{37F1C8EA-B4AD-4B0B-93A2-CC770BDF3372}" name="ID_OBJETO_VALOR" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3EB20B64-F6DD-410D-8178-4BF665C122F3}" name="Tabla4" displayName="Tabla4" ref="A2:B11" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A2:B11" xr:uid="{3EB20B64-F6DD-410D-8178-4BF665C122F3}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E2BFE1D0-31AA-4096-A1A9-1EC1DD7949F4}" name="ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{618BA1C2-FD69-4424-9500-69A5BC1723AC}" name="NOMBRE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,151 +1137,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CBBB6F-8335-48EE-8480-49A90F0FD67D}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="8">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="8">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800419FB-0D8F-4C91-996D-B215BAFBD9A6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1335,12 +1190,267 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E56A2-F0E5-48C0-8BE1-44637F7D6F40}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CBBB6F-8335-48EE-8480-49A90F0FD67D}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="B3:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C56056-1706-433D-8016-D90B33329DC4}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F13" sqref="B3:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,12 +1792,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D36DFC8-5BE2-4975-BB25-A5E0CB36C4A3}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,114 +2395,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2E56A2-F0E5-48C0-8BE1-44637F7D6F40}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>